<commit_message>
tampa sat back to kd
</commit_message>
<xml_diff>
--- a/word_revision/Table1.xlsx
+++ b/word_revision/Table1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\docs\manuscripts\sgdepth_manu\word\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\docs\manuscripts\sgdepth_manu\word_revision\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>OTB</t>
   </si>
@@ -91,12 +91,6 @@
     </r>
   </si>
   <si>
-    <t>BB: http://atoll.floridamarine.org/Data/metadata/SDE Current/seagrass bigbend 2006 poly.htm</t>
-  </si>
-  <si>
-    <t>OTB: http://www.swfwmd.state.fl.us/data/gis/layer library/category/swim</t>
-  </si>
-  <si>
     <t>UIRL: http://www.sjrwmd.com/gisdevelopment/docs/themes.html</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
     </r>
   </si>
   <si>
-    <t>WCB: http://atoll.floridamarine.org/data/metadata/SDE Current/seagrass chotawhatchee 2007 poly.htm</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -166,11 +157,17 @@
       <t xml:space="preserve"> Characteristics of coastal segments used to evaluate seagrass depth of colonization estimates (see Fig. 2 for spatial distribution).  Year is the date of the seagrass coverage and bathymetric data.  Latitude and longitude are the geographic centers of each segment.  Area and depth values are square kilometers and meters, respectively.  Secchi measurements (m) were obtained from the Florida Department of Environmental Protection's Impaired Waters Rule (IWR) database, update number 40.  Secchi mean and standard errors are based on all observations within the ten years preceding each seagrass survey</t>
     </r>
   </si>
+  <si>
+    <t>OTB: http://data.swfwmd.opendata.arcgis.com/</t>
+  </si>
+  <si>
+    <t>BB, WCB: http://geodata.myfwc.com/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -283,10 +280,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -382,6 +379,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -417,6 +431,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -569,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="A16" sqref="A16:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -583,13 +614,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="A1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
@@ -761,7 +792,7 @@
     </row>
     <row r="12" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -770,16 +801,16 @@
     </row>
     <row r="13" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -788,7 +819,7 @@
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -797,25 +828,15 @@
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A17:E17"/>
+  <mergeCells count="6">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A13:E13"/>

</xml_diff>

<commit_message>
working on ESCO revisions take 2
</commit_message>
<xml_diff>
--- a/word_revision/Table1.xlsx
+++ b/word_revision/Table1.xlsx
@@ -59,83 +59,7 @@
     <t>Secchi (se)</t>
   </si>
   <si>
-    <r>
-      <t>BB</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>a</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Year</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>b</t>
-    </r>
-  </si>
-  <si>
     <t>UIRL: http://www.sjrwmd.com/gisdevelopment/docs/themes.html</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>BB: Big Bend, OTB: Old Tampa Bay, UIRL: Upper Indian R. Lagoon, WCB: Western Choctawhatchee Bay</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>b</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>Seagrass coverage data sources, see methods for bathymetry data sources</t>
-    </r>
   </si>
   <si>
     <r>
@@ -163,12 +87,24 @@
   <si>
     <t>BB, WCB: http://geodata.myfwc.com/</t>
   </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>BB: Big Bend, OTB: Old Tampa Bay, UIRL: Upper Indian R. Lagoon, WCB: Western Choctawhatchee Bay</t>
+  </si>
+  <si>
+    <t>Seagrass coverage data sources, see methods for bathymetry data sources</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,22 +119,6 @@
       <family val="1"/>
     </font>
     <font>
-      <i/>
-      <vertAlign val="superscript"/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <i/>
-      <vertAlign val="superscript"/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Times"/>
@@ -277,14 +197,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -603,7 +523,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:E16"/>
+      <selection activeCell="A14" sqref="A14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -614,18 +534,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-    </row>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>0</v>
@@ -637,9 +557,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4">
         <v>2006</v>
@@ -791,58 +711,58 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="A15" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="A16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A16:E16"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>